<commit_message>
updated group project specifications
</commit_message>
<xml_diff>
--- a/Documentation/Gantt_Chart_Template.xlsx
+++ b/Documentation/Gantt_Chart_Template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E30FD7B-FE22-41C1-8AE7-A8B1DE8F1B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{3E30FD7B-FE22-41C1-8AE7-A8B1DE8F1B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52B7EC9C-160C-4A67-A260-2F1AA5D4BDEC}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="26895" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -39,10 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
-  <si>
-    <t>Phase 1 Title</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
   <si>
     <t>Task 3</t>
   </si>
@@ -75,9 +72,6 @@
 TO</t>
   </si>
   <si>
-    <t>PROJECT TITLE</t>
-  </si>
-  <si>
     <t>Project Management Templates</t>
   </si>
   <si>
@@ -136,12 +130,6 @@
   </si>
   <si>
     <t>Click on the link below to visit vertex42.com and learn more about how to use this template, such as how to calculate days and work days, create task dependencies, change the colors of the bars, add a scroll bar to make it easier to change the display week, extend the date range displayed in the chart, etc.</t>
-  </si>
-  <si>
-    <t>Company Name</t>
-  </si>
-  <si>
-    <t>Project Lead</t>
   </si>
   <si>
     <t>There are 2 worksheets in this workbook. 
@@ -159,9 +147,6 @@
   </si>
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>Name</t>
   </si>
   <si>
     <t>Sample phase title block</t>
@@ -235,6 +220,39 @@
 Continue navigating down column A cells to learn more.
 If you haven't added any new rows in this worksheet, you will find 2 additional sample phase blocks have been created for you in cells B20 and B26. Otherwise, navigate through column A cells to find the additional blocks. 
 Repeat the instructions from cells A8 and A9 whenever you need to.</t>
+  </si>
+  <si>
+    <t>GroceryGrove</t>
+  </si>
+  <si>
+    <t>WebDemons</t>
+  </si>
+  <si>
+    <t>Attiyah and Priyansh</t>
+  </si>
+  <si>
+    <t>Initaial Set-up</t>
+  </si>
+  <si>
+    <t>Clone Git Repo</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>Priyansh</t>
+  </si>
+  <si>
+    <t>Edit Group Norms</t>
+  </si>
+  <si>
+    <t>Edit Project Specification document</t>
+  </si>
+  <si>
+    <t>Attiyah</t>
+  </si>
+  <si>
+    <t>finish all initial documentations</t>
   </si>
 </sst>
 </file>
@@ -248,7 +266,7 @@
     <numFmt numFmtId="166" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="167" formatCode="d"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,6 +427,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -645,7 +671,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -886,6 +912,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="12">
       <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1206,6 +1235,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1472,33 +1505,33 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL36"/>
+  <dimension ref="A1:BL35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="58" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="64" width="2.5703125" customWidth="1"/>
-    <col min="69" max="70" width="10.28515625"/>
+    <col min="1" max="1" width="2.7265625" style="58" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" customWidth="1"/>
+    <col min="7" max="7" width="2.7265625" customWidth="1"/>
+    <col min="8" max="8" width="6.1796875" hidden="1" customWidth="1"/>
+    <col min="9" max="64" width="2.54296875" customWidth="1"/>
+    <col min="69" max="70" width="10.26953125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A1" s="59" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B1" s="63" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1506,386 +1539,386 @@
       <c r="F1" s="47"/>
       <c r="H1" s="2"/>
       <c r="I1" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="58" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B2" s="64" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="I2" s="61" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="58" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="89" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="90"/>
-      <c r="E3" s="88">
+        <v>49</v>
+      </c>
+      <c r="C3" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="91"/>
+      <c r="E3" s="89">
         <f ca="1">TODAY()</f>
-        <v>45419</v>
-      </c>
-      <c r="F3" s="88"/>
-    </row>
-    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45429</v>
+      </c>
+      <c r="F3" s="89"/>
+    </row>
+    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="59" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="89" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="90"/>
+        <v>40</v>
+      </c>
+      <c r="C4" s="90" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="91"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="85">
+      <c r="I4" s="86">
         <f ca="1">I5</f>
-        <v>45418</v>
-      </c>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="85">
+        <v>45425</v>
+      </c>
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="88"/>
+      <c r="P4" s="86">
         <f ca="1">P5</f>
-        <v>45425</v>
-      </c>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="87"/>
-      <c r="W4" s="85">
+        <v>45432</v>
+      </c>
+      <c r="Q4" s="87"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="87"/>
+      <c r="T4" s="87"/>
+      <c r="U4" s="87"/>
+      <c r="V4" s="88"/>
+      <c r="W4" s="86">
         <f ca="1">W5</f>
-        <v>45432</v>
-      </c>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="86"/>
-      <c r="Z4" s="86"/>
-      <c r="AA4" s="86"/>
-      <c r="AB4" s="86"/>
-      <c r="AC4" s="87"/>
-      <c r="AD4" s="85">
+        <v>45439</v>
+      </c>
+      <c r="X4" s="87"/>
+      <c r="Y4" s="87"/>
+      <c r="Z4" s="87"/>
+      <c r="AA4" s="87"/>
+      <c r="AB4" s="87"/>
+      <c r="AC4" s="88"/>
+      <c r="AD4" s="86">
         <f ca="1">AD5</f>
-        <v>45439</v>
-      </c>
-      <c r="AE4" s="86"/>
-      <c r="AF4" s="86"/>
-      <c r="AG4" s="86"/>
-      <c r="AH4" s="86"/>
-      <c r="AI4" s="86"/>
-      <c r="AJ4" s="87"/>
-      <c r="AK4" s="85">
+        <v>45446</v>
+      </c>
+      <c r="AE4" s="87"/>
+      <c r="AF4" s="87"/>
+      <c r="AG4" s="87"/>
+      <c r="AH4" s="87"/>
+      <c r="AI4" s="87"/>
+      <c r="AJ4" s="88"/>
+      <c r="AK4" s="86">
         <f ca="1">AK5</f>
-        <v>45446</v>
-      </c>
-      <c r="AL4" s="86"/>
-      <c r="AM4" s="86"/>
-      <c r="AN4" s="86"/>
-      <c r="AO4" s="86"/>
-      <c r="AP4" s="86"/>
-      <c r="AQ4" s="87"/>
-      <c r="AR4" s="85">
+        <v>45453</v>
+      </c>
+      <c r="AL4" s="87"/>
+      <c r="AM4" s="87"/>
+      <c r="AN4" s="87"/>
+      <c r="AO4" s="87"/>
+      <c r="AP4" s="87"/>
+      <c r="AQ4" s="88"/>
+      <c r="AR4" s="86">
         <f ca="1">AR5</f>
-        <v>45453</v>
-      </c>
-      <c r="AS4" s="86"/>
-      <c r="AT4" s="86"/>
-      <c r="AU4" s="86"/>
-      <c r="AV4" s="86"/>
-      <c r="AW4" s="86"/>
-      <c r="AX4" s="87"/>
-      <c r="AY4" s="85">
+        <v>45460</v>
+      </c>
+      <c r="AS4" s="87"/>
+      <c r="AT4" s="87"/>
+      <c r="AU4" s="87"/>
+      <c r="AV4" s="87"/>
+      <c r="AW4" s="87"/>
+      <c r="AX4" s="88"/>
+      <c r="AY4" s="86">
         <f ca="1">AY5</f>
-        <v>45460</v>
-      </c>
-      <c r="AZ4" s="86"/>
-      <c r="BA4" s="86"/>
-      <c r="BB4" s="86"/>
-      <c r="BC4" s="86"/>
-      <c r="BD4" s="86"/>
-      <c r="BE4" s="87"/>
-      <c r="BF4" s="85">
+        <v>45467</v>
+      </c>
+      <c r="AZ4" s="87"/>
+      <c r="BA4" s="87"/>
+      <c r="BB4" s="87"/>
+      <c r="BC4" s="87"/>
+      <c r="BD4" s="87"/>
+      <c r="BE4" s="88"/>
+      <c r="BF4" s="86">
         <f ca="1">BF5</f>
-        <v>45467</v>
-      </c>
-      <c r="BG4" s="86"/>
-      <c r="BH4" s="86"/>
-      <c r="BI4" s="86"/>
-      <c r="BJ4" s="86"/>
-      <c r="BK4" s="86"/>
-      <c r="BL4" s="87"/>
-    </row>
-    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45474</v>
+      </c>
+      <c r="BG4" s="87"/>
+      <c r="BH4" s="87"/>
+      <c r="BI4" s="87"/>
+      <c r="BJ4" s="87"/>
+      <c r="BK4" s="87"/>
+      <c r="BL4" s="88"/>
+    </row>
+    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
+        <v>41</v>
+      </c>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>45418</v>
+        <v>45425</v>
       </c>
       <c r="J5" s="10">
         <f ca="1">I5+1</f>
-        <v>45419</v>
+        <v>45426</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>45420</v>
+        <v>45427</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45421</v>
+        <v>45428</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45422</v>
+        <v>45429</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45423</v>
+        <v>45430</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45424</v>
+        <v>45431</v>
       </c>
       <c r="P5" s="11">
         <f ca="1">O5+1</f>
-        <v>45425</v>
+        <v>45432</v>
       </c>
       <c r="Q5" s="10">
         <f ca="1">P5+1</f>
-        <v>45426</v>
+        <v>45433</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45427</v>
+        <v>45434</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45428</v>
+        <v>45435</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45429</v>
+        <v>45436</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45430</v>
+        <v>45437</v>
       </c>
       <c r="V5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45431</v>
+        <v>45438</v>
       </c>
       <c r="W5" s="11">
         <f ca="1">V5+1</f>
-        <v>45432</v>
+        <v>45439</v>
       </c>
       <c r="X5" s="10">
         <f ca="1">W5+1</f>
-        <v>45433</v>
+        <v>45440</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45434</v>
+        <v>45441</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45435</v>
+        <v>45442</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45436</v>
+        <v>45443</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45437</v>
+        <v>45444</v>
       </c>
       <c r="AC5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45438</v>
+        <v>45445</v>
       </c>
       <c r="AD5" s="11">
         <f ca="1">AC5+1</f>
-        <v>45439</v>
+        <v>45446</v>
       </c>
       <c r="AE5" s="10">
         <f ca="1">AD5+1</f>
-        <v>45440</v>
+        <v>45447</v>
       </c>
       <c r="AF5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45441</v>
+        <v>45448</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45442</v>
+        <v>45449</v>
       </c>
       <c r="AH5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45443</v>
+        <v>45450</v>
       </c>
       <c r="AI5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45444</v>
+        <v>45451</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45445</v>
+        <v>45452</v>
       </c>
       <c r="AK5" s="11">
         <f ca="1">AJ5+1</f>
-        <v>45446</v>
+        <v>45453</v>
       </c>
       <c r="AL5" s="10">
         <f ca="1">AK5+1</f>
-        <v>45447</v>
+        <v>45454</v>
       </c>
       <c r="AM5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45448</v>
+        <v>45455</v>
       </c>
       <c r="AN5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45449</v>
+        <v>45456</v>
       </c>
       <c r="AO5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45450</v>
+        <v>45457</v>
       </c>
       <c r="AP5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45451</v>
+        <v>45458</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45452</v>
+        <v>45459</v>
       </c>
       <c r="AR5" s="11">
         <f ca="1">AQ5+1</f>
-        <v>45453</v>
+        <v>45460</v>
       </c>
       <c r="AS5" s="10">
         <f ca="1">AR5+1</f>
-        <v>45454</v>
+        <v>45461</v>
       </c>
       <c r="AT5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45455</v>
+        <v>45462</v>
       </c>
       <c r="AU5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="AV5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="AW5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="AY5" s="11">
         <f ca="1">AX5+1</f>
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="AZ5" s="10">
         <f ca="1">AY5+1</f>
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="BA5" s="10">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>45462</v>
+        <v>45469</v>
       </c>
       <c r="BB5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45463</v>
+        <v>45470</v>
       </c>
       <c r="BC5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45464</v>
+        <v>45471</v>
       </c>
       <c r="BD5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45465</v>
+        <v>45472</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" ca="1" si="1"/>
-        <v>45466</v>
+        <v>45473</v>
       </c>
       <c r="BF5" s="11">
         <f ca="1">BE5+1</f>
-        <v>45467</v>
+        <v>45474</v>
       </c>
       <c r="BG5" s="10">
         <f ca="1">BF5+1</f>
-        <v>45468</v>
+        <v>45475</v>
       </c>
       <c r="BH5" s="10">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>45469</v>
+        <v>45476</v>
       </c>
       <c r="BI5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45470</v>
+        <v>45477</v>
       </c>
       <c r="BJ5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45471</v>
+        <v>45478</v>
       </c>
       <c r="BK5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45472</v>
+        <v>45479</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" ca="1" si="2"/>
-        <v>45473</v>
-      </c>
-    </row>
-    <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45480</v>
+      </c>
+    </row>
+    <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="59" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I6" s="13" t="str">
         <f t="shared" ref="I6" ca="1" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
@@ -2112,9 +2145,9 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="58" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C7" s="62"/>
       <c r="E7"/>
@@ -2179,12 +2212,12 @@
       <c r="BK7" s="44"/>
       <c r="BL7" s="44"/>
     </row>
-    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="59" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C8" s="71"/>
       <c r="D8" s="19"/>
@@ -2192,7 +2225,7 @@
       <c r="F8" s="21"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17" t="str">
-        <f t="shared" ref="H8:H33" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H32" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="44"/>
@@ -2252,31 +2285,31 @@
       <c r="BK8" s="44"/>
       <c r="BL8" s="44"/>
     </row>
-    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="59" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B9" s="80" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="72" t="s">
-        <v>38</v>
+        <v>51</v>
+      </c>
+      <c r="C9" s="85" t="s">
+        <v>52</v>
       </c>
       <c r="D9" s="22">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E9" s="66">
         <f ca="1">Project_Start</f>
-        <v>45419</v>
+        <v>45429</v>
       </c>
       <c r="F9" s="66">
-        <f ca="1">E9+3</f>
-        <v>45422</v>
+        <f ca="1">Project_Start</f>
+        <v>45429</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I9" s="44"/>
       <c r="J9" s="44"/>
@@ -2335,24 +2368,26 @@
       <c r="BK9" s="44"/>
       <c r="BL9" s="44"/>
     </row>
-    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="59" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B10" s="80" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="72"/>
+        <v>54</v>
+      </c>
+      <c r="C10" s="72" t="s">
+        <v>53</v>
+      </c>
       <c r="D10" s="22">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E10" s="66">
         <f ca="1">F9</f>
-        <v>45422</v>
+        <v>45429</v>
       </c>
       <c r="F10" s="66">
         <f ca="1">E10+2</f>
-        <v>45424</v>
+        <v>45431</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17">
@@ -2416,22 +2451,24 @@
       <c r="BK10" s="44"/>
       <c r="BL10" s="44"/>
     </row>
-    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="58"/>
       <c r="B11" s="80" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="72"/>
+        <v>55</v>
+      </c>
+      <c r="C11" s="72" t="s">
+        <v>56</v>
+      </c>
       <c r="D11" s="22">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E11" s="66">
         <f ca="1">F10</f>
-        <v>45424</v>
+        <v>45431</v>
       </c>
       <c r="F11" s="66">
         <f ca="1">E11+4</f>
-        <v>45428</v>
+        <v>45435</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17">
@@ -2495,22 +2532,24 @@
       <c r="BK11" s="44"/>
       <c r="BL11" s="44"/>
     </row>
-    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="58"/>
       <c r="B12" s="80" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="72"/>
+        <v>57</v>
+      </c>
+      <c r="C12" s="72" t="s">
+        <v>52</v>
+      </c>
       <c r="D12" s="22">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="E12" s="66">
-        <f ca="1">F11</f>
-        <v>45428</v>
+        <f ca="1">F9</f>
+        <v>45429</v>
       </c>
       <c r="F12" s="66">
         <f ca="1">E12+5</f>
-        <v>45433</v>
+        <v>45434</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="17">
@@ -2574,25 +2613,21 @@
       <c r="BK12" s="44"/>
       <c r="BL12" s="44"/>
     </row>
-    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="58"/>
-      <c r="B13" s="80" t="s">
+    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="72"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="66">
-        <f ca="1">E10+1</f>
-        <v>45423</v>
-      </c>
-      <c r="F13" s="66">
-        <f ca="1">E13+2</f>
-        <v>45425</v>
-      </c>
+      <c r="C13" s="73"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="17"/>
-      <c r="H13" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+      <c r="H13" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="I13" s="44"/>
       <c r="J13" s="44"/>
@@ -2651,21 +2686,27 @@
       <c r="BK13" s="44"/>
       <c r="BL13" s="44"/>
     </row>
-    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="59" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="23" t="s">
+    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="59"/>
+      <c r="B14" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="73"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="67" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F14" s="67" t="e">
+        <f>E14+4</f>
+        <v>#REF!</v>
+      </c>
       <c r="G14" s="17"/>
-      <c r="H14" s="17" t="str">
+      <c r="H14" s="17" t="e">
         <f t="shared" si="6"/>
-        <v/>
+        <v>#REF!</v>
       </c>
       <c r="I14" s="44"/>
       <c r="J14" s="44"/>
@@ -2724,8 +2765,8 @@
       <c r="BK14" s="44"/>
       <c r="BL14" s="44"/>
     </row>
-    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="59"/>
+    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="58"/>
       <c r="B15" s="81" t="s">
         <v>5</v>
       </c>
@@ -2733,18 +2774,18 @@
       <c r="D15" s="27">
         <v>0.5</v>
       </c>
-      <c r="E15" s="67">
-        <f ca="1">E13+1</f>
-        <v>45424</v>
-      </c>
-      <c r="F15" s="67">
-        <f ca="1">E15+4</f>
-        <v>45428</v>
+      <c r="E15" s="67" t="e">
+        <f>E14+2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F15" s="67" t="e">
+        <f>E15+5</f>
+        <v>#REF!</v>
       </c>
       <c r="G15" s="17"/>
-      <c r="H15" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+      <c r="H15" s="17" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
       </c>
       <c r="I15" s="44"/>
       <c r="J15" s="44"/>
@@ -2758,8 +2799,8 @@
       <c r="R15" s="44"/>
       <c r="S15" s="44"/>
       <c r="T15" s="44"/>
-      <c r="U15" s="44"/>
-      <c r="V15" s="44"/>
+      <c r="U15" s="45"/>
+      <c r="V15" s="45"/>
       <c r="W15" s="44"/>
       <c r="X15" s="44"/>
       <c r="Y15" s="44"/>
@@ -2803,27 +2844,25 @@
       <c r="BK15" s="44"/>
       <c r="BL15" s="44"/>
     </row>
-    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="58"/>
       <c r="B16" s="81" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C16" s="74"/>
-      <c r="D16" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="E16" s="67">
-        <f ca="1">E15+2</f>
-        <v>45426</v>
-      </c>
-      <c r="F16" s="67">
-        <f ca="1">E16+5</f>
-        <v>45431</v>
+      <c r="D16" s="27"/>
+      <c r="E16" s="67" t="e">
+        <f>F15</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F16" s="67" t="e">
+        <f>E16+3</f>
+        <v>#REF!</v>
       </c>
       <c r="G16" s="17"/>
-      <c r="H16" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>6</v>
+      <c r="H16" s="17" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
       </c>
       <c r="I16" s="44"/>
       <c r="J16" s="44"/>
@@ -2837,8 +2876,8 @@
       <c r="R16" s="44"/>
       <c r="S16" s="44"/>
       <c r="T16" s="44"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="45"/>
+      <c r="U16" s="44"/>
+      <c r="V16" s="44"/>
       <c r="W16" s="44"/>
       <c r="X16" s="44"/>
       <c r="Y16" s="44"/>
@@ -2882,25 +2921,25 @@
       <c r="BK16" s="44"/>
       <c r="BL16" s="44"/>
     </row>
-    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="58"/>
       <c r="B17" s="81" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="74"/>
       <c r="D17" s="27"/>
-      <c r="E17" s="67">
-        <f ca="1">F16</f>
-        <v>45431</v>
-      </c>
-      <c r="F17" s="67">
-        <f ca="1">E17+3</f>
-        <v>45434</v>
+      <c r="E17" s="67" t="e">
+        <f>E16</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F17" s="67" t="e">
+        <f>E17+2</f>
+        <v>#REF!</v>
       </c>
       <c r="G17" s="17"/>
-      <c r="H17" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+      <c r="H17" s="17" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
       </c>
       <c r="I17" s="44"/>
       <c r="J17" s="44"/>
@@ -2918,7 +2957,7 @@
       <c r="V17" s="44"/>
       <c r="W17" s="44"/>
       <c r="X17" s="44"/>
-      <c r="Y17" s="44"/>
+      <c r="Y17" s="45"/>
       <c r="Z17" s="44"/>
       <c r="AA17" s="44"/>
       <c r="AB17" s="44"/>
@@ -2959,25 +2998,25 @@
       <c r="BK17" s="44"/>
       <c r="BL17" s="44"/>
     </row>
-    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="58"/>
       <c r="B18" s="81" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="74"/>
       <c r="D18" s="27"/>
-      <c r="E18" s="67">
-        <f ca="1">E17</f>
-        <v>45431</v>
-      </c>
-      <c r="F18" s="67">
-        <f ca="1">E18+2</f>
-        <v>45433</v>
+      <c r="E18" s="67" t="e">
+        <f>E17</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F18" s="67" t="e">
+        <f>E18+3</f>
+        <v>#REF!</v>
       </c>
       <c r="G18" s="17"/>
-      <c r="H18" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+      <c r="H18" s="17" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
       </c>
       <c r="I18" s="44"/>
       <c r="J18" s="44"/>
@@ -2995,7 +3034,7 @@
       <c r="V18" s="44"/>
       <c r="W18" s="44"/>
       <c r="X18" s="44"/>
-      <c r="Y18" s="45"/>
+      <c r="Y18" s="44"/>
       <c r="Z18" s="44"/>
       <c r="AA18" s="44"/>
       <c r="AB18" s="44"/>
@@ -3036,25 +3075,21 @@
       <c r="BK18" s="44"/>
       <c r="BL18" s="44"/>
     </row>
-    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="58"/>
-      <c r="B19" s="81" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="74"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="67">
-        <f ca="1">E18</f>
-        <v>45431</v>
-      </c>
-      <c r="F19" s="67">
-        <f ca="1">E19+3</f>
-        <v>45434</v>
-      </c>
+    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="75"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="31"/>
       <c r="G19" s="17"/>
-      <c r="H19" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+      <c r="H19" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="I19" s="44"/>
       <c r="J19" s="44"/>
@@ -3113,21 +3148,25 @@
       <c r="BK19" s="44"/>
       <c r="BL19" s="44"/>
     </row>
-    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="75"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="31"/>
+    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="58"/>
+      <c r="B20" s="82" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="76"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="68">
+        <f ca="1">E9+15</f>
+        <v>45444</v>
+      </c>
+      <c r="F20" s="68">
+        <f ca="1">E20+5</f>
+        <v>45449</v>
+      </c>
       <c r="G20" s="17"/>
-      <c r="H20" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+      <c r="H20" s="17">
+        <f t="shared" ca="1" si="6"/>
+        <v>6</v>
       </c>
       <c r="I20" s="44"/>
       <c r="J20" s="44"/>
@@ -3186,7 +3225,7 @@
       <c r="BK20" s="44"/>
       <c r="BL20" s="44"/>
     </row>
-    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="58"/>
       <c r="B21" s="82" t="s">
         <v>5</v>
@@ -3194,17 +3233,17 @@
       <c r="C21" s="76"/>
       <c r="D21" s="32"/>
       <c r="E21" s="68">
-        <f ca="1">E9+15</f>
-        <v>45434</v>
+        <f ca="1">F20+1</f>
+        <v>45450</v>
       </c>
       <c r="F21" s="68">
-        <f ca="1">E21+5</f>
-        <v>45439</v>
+        <f ca="1">E21+4</f>
+        <v>45454</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I21" s="44"/>
       <c r="J21" s="44"/>
@@ -3263,25 +3302,25 @@
       <c r="BK21" s="44"/>
       <c r="BL21" s="44"/>
     </row>
-    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="58"/>
       <c r="B22" s="82" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C22" s="76"/>
       <c r="D22" s="32"/>
       <c r="E22" s="68">
-        <f ca="1">F21+1</f>
-        <v>45440</v>
+        <f ca="1">E21+5</f>
+        <v>45455</v>
       </c>
       <c r="F22" s="68">
-        <f ca="1">E22+4</f>
-        <v>45444</v>
+        <f ca="1">E22+5</f>
+        <v>45460</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I22" s="44"/>
       <c r="J22" s="44"/>
@@ -3340,7 +3379,7 @@
       <c r="BK22" s="44"/>
       <c r="BL22" s="44"/>
     </row>
-    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="58"/>
       <c r="B23" s="82" t="s">
         <v>1</v>
@@ -3348,17 +3387,17 @@
       <c r="C23" s="76"/>
       <c r="D23" s="32"/>
       <c r="E23" s="68">
-        <f ca="1">E22+5</f>
-        <v>45445</v>
+        <f ca="1">F22+1</f>
+        <v>45461</v>
       </c>
       <c r="F23" s="68">
-        <f ca="1">E23+5</f>
-        <v>45450</v>
+        <f ca="1">E23+4</f>
+        <v>45465</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17">
         <f t="shared" ca="1" si="6"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I23" s="44"/>
       <c r="J23" s="44"/>
@@ -3417,7 +3456,7 @@
       <c r="BK23" s="44"/>
       <c r="BL23" s="44"/>
     </row>
-    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="58"/>
       <c r="B24" s="82" t="s">
         <v>2</v>
@@ -3425,12 +3464,12 @@
       <c r="C24" s="76"/>
       <c r="D24" s="32"/>
       <c r="E24" s="68">
-        <f ca="1">F23+1</f>
-        <v>45451</v>
+        <f ca="1">E22</f>
+        <v>45455</v>
       </c>
       <c r="F24" s="68">
         <f ca="1">E24+4</f>
-        <v>45455</v>
+        <v>45459</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="17">
@@ -3494,25 +3533,21 @@
       <c r="BK24" s="44"/>
       <c r="BL24" s="44"/>
     </row>
-    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="58"/>
-      <c r="B25" s="82" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="76"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="68">
-        <f ca="1">E23</f>
-        <v>45445</v>
-      </c>
-      <c r="F25" s="68">
-        <f ca="1">E25+4</f>
-        <v>45449</v>
-      </c>
+    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="77"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="36"/>
       <c r="G25" s="17"/>
-      <c r="H25" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+      <c r="H25" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="I25" s="44"/>
       <c r="J25" s="44"/>
@@ -3571,21 +3606,23 @@
       <c r="BK25" s="44"/>
       <c r="BL25" s="44"/>
     </row>
-    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="36"/>
+    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="58"/>
+      <c r="B26" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="78"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="69" t="s">
+        <v>33</v>
+      </c>
       <c r="G26" s="17"/>
-      <c r="H26" s="17" t="str">
+      <c r="H26" s="17" t="e">
         <f t="shared" si="6"/>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="I26" s="44"/>
       <c r="J26" s="44"/>
@@ -3644,7 +3681,7 @@
       <c r="BK26" s="44"/>
       <c r="BL26" s="44"/>
     </row>
-    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="58"/>
       <c r="B27" s="83" t="s">
         <v>5</v>
@@ -3652,10 +3689,10 @@
       <c r="C27" s="78"/>
       <c r="D27" s="37"/>
       <c r="E27" s="69" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F27" s="69" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="17" t="e">
@@ -3719,18 +3756,18 @@
       <c r="BK27" s="44"/>
       <c r="BL27" s="44"/>
     </row>
-    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="58"/>
       <c r="B28" s="83" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C28" s="78"/>
       <c r="D28" s="37"/>
       <c r="E28" s="69" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F28" s="69" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="17" t="e">
@@ -3794,7 +3831,7 @@
       <c r="BK28" s="44"/>
       <c r="BL28" s="44"/>
     </row>
-    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="58"/>
       <c r="B29" s="83" t="s">
         <v>1</v>
@@ -3802,10 +3839,10 @@
       <c r="C29" s="78"/>
       <c r="D29" s="37"/>
       <c r="E29" s="69" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F29" s="69" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="17" t="e">
@@ -3869,7 +3906,7 @@
       <c r="BK29" s="44"/>
       <c r="BL29" s="44"/>
     </row>
-    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="58"/>
       <c r="B30" s="83" t="s">
         <v>2</v>
@@ -3877,10 +3914,10 @@
       <c r="C30" s="78"/>
       <c r="D30" s="37"/>
       <c r="E30" s="69" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F30" s="69" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="17" t="e">
@@ -3944,23 +3981,19 @@
       <c r="BK30" s="44"/>
       <c r="BL30" s="44"/>
     </row>
-    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="58"/>
-      <c r="B31" s="83" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="78"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="69" t="s">
-        <v>37</v>
-      </c>
-      <c r="F31" s="69" t="s">
-        <v>37</v>
-      </c>
+    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="58" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="84"/>
+      <c r="C31" s="79"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
       <c r="G31" s="17"/>
-      <c r="H31" s="17" t="e">
+      <c r="H31" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="I31" s="44"/>
       <c r="J31" s="44"/>
@@ -4019,159 +4052,88 @@
       <c r="BK31" s="44"/>
       <c r="BL31" s="44"/>
     </row>
-    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="58" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="84"/>
-      <c r="C32" s="79"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="70"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17" t="str">
+    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="39"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I32" s="44"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="44"/>
-      <c r="L32" s="44"/>
-      <c r="M32" s="44"/>
-      <c r="N32" s="44"/>
-      <c r="O32" s="44"/>
-      <c r="P32" s="44"/>
-      <c r="Q32" s="44"/>
-      <c r="R32" s="44"/>
-      <c r="S32" s="44"/>
-      <c r="T32" s="44"/>
-      <c r="U32" s="44"/>
-      <c r="V32" s="44"/>
-      <c r="W32" s="44"/>
-      <c r="X32" s="44"/>
-      <c r="Y32" s="44"/>
-      <c r="Z32" s="44"/>
-      <c r="AA32" s="44"/>
-      <c r="AB32" s="44"/>
-      <c r="AC32" s="44"/>
-      <c r="AD32" s="44"/>
-      <c r="AE32" s="44"/>
-      <c r="AF32" s="44"/>
-      <c r="AG32" s="44"/>
-      <c r="AH32" s="44"/>
-      <c r="AI32" s="44"/>
-      <c r="AJ32" s="44"/>
-      <c r="AK32" s="44"/>
-      <c r="AL32" s="44"/>
-      <c r="AM32" s="44"/>
-      <c r="AN32" s="44"/>
-      <c r="AO32" s="44"/>
-      <c r="AP32" s="44"/>
-      <c r="AQ32" s="44"/>
-      <c r="AR32" s="44"/>
-      <c r="AS32" s="44"/>
-      <c r="AT32" s="44"/>
-      <c r="AU32" s="44"/>
-      <c r="AV32" s="44"/>
-      <c r="AW32" s="44"/>
-      <c r="AX32" s="44"/>
-      <c r="AY32" s="44"/>
-      <c r="AZ32" s="44"/>
-      <c r="BA32" s="44"/>
-      <c r="BB32" s="44"/>
-      <c r="BC32" s="44"/>
-      <c r="BD32" s="44"/>
-      <c r="BE32" s="44"/>
-      <c r="BF32" s="44"/>
-      <c r="BG32" s="44"/>
-      <c r="BH32" s="44"/>
-      <c r="BI32" s="44"/>
-      <c r="BJ32" s="44"/>
-      <c r="BK32" s="44"/>
-      <c r="BL32" s="44"/>
-    </row>
-    <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="59" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="46"/>
-      <c r="N33" s="46"/>
-      <c r="O33" s="46"/>
-      <c r="P33" s="46"/>
-      <c r="Q33" s="46"/>
-      <c r="R33" s="46"/>
-      <c r="S33" s="46"/>
-      <c r="T33" s="46"/>
-      <c r="U33" s="46"/>
-      <c r="V33" s="46"/>
-      <c r="W33" s="46"/>
-      <c r="X33" s="46"/>
-      <c r="Y33" s="46"/>
-      <c r="Z33" s="46"/>
-      <c r="AA33" s="46"/>
-      <c r="AB33" s="46"/>
-      <c r="AC33" s="46"/>
-      <c r="AD33" s="46"/>
-      <c r="AE33" s="46"/>
-      <c r="AF33" s="46"/>
-      <c r="AG33" s="46"/>
-      <c r="AH33" s="46"/>
-      <c r="AI33" s="46"/>
-      <c r="AJ33" s="46"/>
-      <c r="AK33" s="46"/>
-      <c r="AL33" s="46"/>
-      <c r="AM33" s="46"/>
-      <c r="AN33" s="46"/>
-      <c r="AO33" s="46"/>
-      <c r="AP33" s="46"/>
-      <c r="AQ33" s="46"/>
-      <c r="AR33" s="46"/>
-      <c r="AS33" s="46"/>
-      <c r="AT33" s="46"/>
-      <c r="AU33" s="46"/>
-      <c r="AV33" s="46"/>
-      <c r="AW33" s="46"/>
-      <c r="AX33" s="46"/>
-      <c r="AY33" s="46"/>
-      <c r="AZ33" s="46"/>
-      <c r="BA33" s="46"/>
-      <c r="BB33" s="46"/>
-      <c r="BC33" s="46"/>
-      <c r="BD33" s="46"/>
-      <c r="BE33" s="46"/>
-      <c r="BF33" s="46"/>
-      <c r="BG33" s="46"/>
-      <c r="BH33" s="46"/>
-      <c r="BI33" s="46"/>
-      <c r="BJ33" s="46"/>
-      <c r="BK33" s="46"/>
-      <c r="BL33" s="46"/>
-    </row>
-    <row r="34" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G34" s="6"/>
-    </row>
-    <row r="35" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="14"/>
-      <c r="F35" s="60"/>
-    </row>
-    <row r="36" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="15"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
+      <c r="N32" s="46"/>
+      <c r="O32" s="46"/>
+      <c r="P32" s="46"/>
+      <c r="Q32" s="46"/>
+      <c r="R32" s="46"/>
+      <c r="S32" s="46"/>
+      <c r="T32" s="46"/>
+      <c r="U32" s="46"/>
+      <c r="V32" s="46"/>
+      <c r="W32" s="46"/>
+      <c r="X32" s="46"/>
+      <c r="Y32" s="46"/>
+      <c r="Z32" s="46"/>
+      <c r="AA32" s="46"/>
+      <c r="AB32" s="46"/>
+      <c r="AC32" s="46"/>
+      <c r="AD32" s="46"/>
+      <c r="AE32" s="46"/>
+      <c r="AF32" s="46"/>
+      <c r="AG32" s="46"/>
+      <c r="AH32" s="46"/>
+      <c r="AI32" s="46"/>
+      <c r="AJ32" s="46"/>
+      <c r="AK32" s="46"/>
+      <c r="AL32" s="46"/>
+      <c r="AM32" s="46"/>
+      <c r="AN32" s="46"/>
+      <c r="AO32" s="46"/>
+      <c r="AP32" s="46"/>
+      <c r="AQ32" s="46"/>
+      <c r="AR32" s="46"/>
+      <c r="AS32" s="46"/>
+      <c r="AT32" s="46"/>
+      <c r="AU32" s="46"/>
+      <c r="AV32" s="46"/>
+      <c r="AW32" s="46"/>
+      <c r="AX32" s="46"/>
+      <c r="AY32" s="46"/>
+      <c r="AZ32" s="46"/>
+      <c r="BA32" s="46"/>
+      <c r="BB32" s="46"/>
+      <c r="BC32" s="46"/>
+      <c r="BD32" s="46"/>
+      <c r="BE32" s="46"/>
+      <c r="BF32" s="46"/>
+      <c r="BG32" s="46"/>
+      <c r="BH32" s="46"/>
+      <c r="BI32" s="46"/>
+      <c r="BJ32" s="46"/>
+      <c r="BK32" s="46"/>
+      <c r="BL32" s="46"/>
+    </row>
+    <row r="33" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="14"/>
+      <c r="F34" s="60"/>
+    </row>
+    <row r="35" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4188,7 +4150,7 @@
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D33">
+  <conditionalFormatting sqref="D7:D32">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4202,12 +4164,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL33">
+  <conditionalFormatting sqref="I5:BL32">
     <cfRule type="expression" dxfId="2" priority="33">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL33">
+  <conditionalFormatting sqref="I7:BL32">
     <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4231,7 +4193,7 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="F18 F22:F23 E23" formula="1"/>
+    <ignoredError sqref="F17 F21:F22 E22" formula="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -4249,7 +4211,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D33</xm:sqref>
+          <xm:sqref>D7:D32</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4263,88 +4225,88 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="87.140625" style="48" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="87.1796875" style="48" customWidth="1"/>
+    <col min="2" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:2" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:2" s="50" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="49"/>
+    </row>
+    <row r="3" spans="1:2" s="54" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="55"/>
+    </row>
+    <row r="4" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+      <c r="A4" s="52" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="53" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="52" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="48" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="57" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+      <c r="A8" s="52" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="58" x14ac:dyDescent="0.3">
+      <c r="A9" s="53" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="48" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="56" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+      <c r="A11" s="52" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.3">
+      <c r="A12" s="53" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="48" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="51" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+      <c r="A14" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="49"/>
-    </row>
-    <row r="3" spans="1:2" s="54" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="55"/>
-    </row>
-    <row r="4" spans="1:2" s="51" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A4" s="52" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="53" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="48" customFormat="1" ht="204.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="51" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A8" s="52" t="s">
+    </row>
+    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="53" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.2">
-      <c r="A9" s="53" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="48" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="51" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A11" s="52" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="53" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="48" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="56" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="51" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A14" s="52" t="s">
+    <row r="16" spans="1:2" ht="72.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="53" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="53" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.2">
-      <c r="A16" s="53" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial template to edit index and products page
</commit_message>
<xml_diff>
--- a/Documentation/Gantt_Chart_Template.xlsx
+++ b/Documentation/Gantt_Chart_Template.xlsx
@@ -916,6 +916,13 @@
     <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -928,13 +935,6 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1508,8 +1508,8 @@
   <dimension ref="A1:BL35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1560,341 +1560,341 @@
       <c r="B3" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="91"/>
-      <c r="E3" s="89">
+      <c r="D3" s="87"/>
+      <c r="E3" s="92">
         <f ca="1">TODAY()</f>
-        <v>45429</v>
-      </c>
-      <c r="F3" s="89"/>
+        <v>45432</v>
+      </c>
+      <c r="F3" s="92"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="90" t="s">
+      <c r="C4" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="91"/>
+      <c r="D4" s="87"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="86">
+      <c r="I4" s="89">
         <f ca="1">I5</f>
-        <v>45425</v>
-      </c>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
-      <c r="M4" s="87"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="86">
+        <v>45432</v>
+      </c>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="89">
         <f ca="1">P5</f>
-        <v>45432</v>
-      </c>
-      <c r="Q4" s="87"/>
-      <c r="R4" s="87"/>
-      <c r="S4" s="87"/>
-      <c r="T4" s="87"/>
-      <c r="U4" s="87"/>
-      <c r="V4" s="88"/>
-      <c r="W4" s="86">
+        <v>45439</v>
+      </c>
+      <c r="Q4" s="90"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="91"/>
+      <c r="W4" s="89">
         <f ca="1">W5</f>
-        <v>45439</v>
-      </c>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
-      <c r="Z4" s="87"/>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="88"/>
-      <c r="AD4" s="86">
+        <v>45446</v>
+      </c>
+      <c r="X4" s="90"/>
+      <c r="Y4" s="90"/>
+      <c r="Z4" s="90"/>
+      <c r="AA4" s="90"/>
+      <c r="AB4" s="90"/>
+      <c r="AC4" s="91"/>
+      <c r="AD4" s="89">
         <f ca="1">AD5</f>
-        <v>45446</v>
-      </c>
-      <c r="AE4" s="87"/>
-      <c r="AF4" s="87"/>
-      <c r="AG4" s="87"/>
-      <c r="AH4" s="87"/>
-      <c r="AI4" s="87"/>
-      <c r="AJ4" s="88"/>
-      <c r="AK4" s="86">
+        <v>45453</v>
+      </c>
+      <c r="AE4" s="90"/>
+      <c r="AF4" s="90"/>
+      <c r="AG4" s="90"/>
+      <c r="AH4" s="90"/>
+      <c r="AI4" s="90"/>
+      <c r="AJ4" s="91"/>
+      <c r="AK4" s="89">
         <f ca="1">AK5</f>
-        <v>45453</v>
-      </c>
-      <c r="AL4" s="87"/>
-      <c r="AM4" s="87"/>
-      <c r="AN4" s="87"/>
-      <c r="AO4" s="87"/>
-      <c r="AP4" s="87"/>
-      <c r="AQ4" s="88"/>
-      <c r="AR4" s="86">
+        <v>45460</v>
+      </c>
+      <c r="AL4" s="90"/>
+      <c r="AM4" s="90"/>
+      <c r="AN4" s="90"/>
+      <c r="AO4" s="90"/>
+      <c r="AP4" s="90"/>
+      <c r="AQ4" s="91"/>
+      <c r="AR4" s="89">
         <f ca="1">AR5</f>
-        <v>45460</v>
-      </c>
-      <c r="AS4" s="87"/>
-      <c r="AT4" s="87"/>
-      <c r="AU4" s="87"/>
-      <c r="AV4" s="87"/>
-      <c r="AW4" s="87"/>
-      <c r="AX4" s="88"/>
-      <c r="AY4" s="86">
+        <v>45467</v>
+      </c>
+      <c r="AS4" s="90"/>
+      <c r="AT4" s="90"/>
+      <c r="AU4" s="90"/>
+      <c r="AV4" s="90"/>
+      <c r="AW4" s="90"/>
+      <c r="AX4" s="91"/>
+      <c r="AY4" s="89">
         <f ca="1">AY5</f>
-        <v>45467</v>
-      </c>
-      <c r="AZ4" s="87"/>
-      <c r="BA4" s="87"/>
-      <c r="BB4" s="87"/>
-      <c r="BC4" s="87"/>
-      <c r="BD4" s="87"/>
-      <c r="BE4" s="88"/>
-      <c r="BF4" s="86">
+        <v>45474</v>
+      </c>
+      <c r="AZ4" s="90"/>
+      <c r="BA4" s="90"/>
+      <c r="BB4" s="90"/>
+      <c r="BC4" s="90"/>
+      <c r="BD4" s="90"/>
+      <c r="BE4" s="91"/>
+      <c r="BF4" s="89">
         <f ca="1">BF5</f>
-        <v>45474</v>
-      </c>
-      <c r="BG4" s="87"/>
-      <c r="BH4" s="87"/>
-      <c r="BI4" s="87"/>
-      <c r="BJ4" s="87"/>
-      <c r="BK4" s="87"/>
-      <c r="BL4" s="88"/>
+        <v>45481</v>
+      </c>
+      <c r="BG4" s="90"/>
+      <c r="BH4" s="90"/>
+      <c r="BI4" s="90"/>
+      <c r="BJ4" s="90"/>
+      <c r="BK4" s="90"/>
+      <c r="BL4" s="91"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>45425</v>
+        <v>45432</v>
       </c>
       <c r="J5" s="10">
         <f ca="1">I5+1</f>
-        <v>45426</v>
+        <v>45433</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>45427</v>
+        <v>45434</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45428</v>
+        <v>45435</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45429</v>
+        <v>45436</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45430</v>
+        <v>45437</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45431</v>
+        <v>45438</v>
       </c>
       <c r="P5" s="11">
         <f ca="1">O5+1</f>
-        <v>45432</v>
+        <v>45439</v>
       </c>
       <c r="Q5" s="10">
         <f ca="1">P5+1</f>
-        <v>45433</v>
+        <v>45440</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45434</v>
+        <v>45441</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45435</v>
+        <v>45442</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45436</v>
+        <v>45443</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45437</v>
+        <v>45444</v>
       </c>
       <c r="V5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45438</v>
+        <v>45445</v>
       </c>
       <c r="W5" s="11">
         <f ca="1">V5+1</f>
-        <v>45439</v>
+        <v>45446</v>
       </c>
       <c r="X5" s="10">
         <f ca="1">W5+1</f>
-        <v>45440</v>
+        <v>45447</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45441</v>
+        <v>45448</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45442</v>
+        <v>45449</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45443</v>
+        <v>45450</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45444</v>
+        <v>45451</v>
       </c>
       <c r="AC5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45445</v>
+        <v>45452</v>
       </c>
       <c r="AD5" s="11">
         <f ca="1">AC5+1</f>
-        <v>45446</v>
+        <v>45453</v>
       </c>
       <c r="AE5" s="10">
         <f ca="1">AD5+1</f>
-        <v>45447</v>
+        <v>45454</v>
       </c>
       <c r="AF5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45448</v>
+        <v>45455</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45449</v>
+        <v>45456</v>
       </c>
       <c r="AH5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45450</v>
+        <v>45457</v>
       </c>
       <c r="AI5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45451</v>
+        <v>45458</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45452</v>
+        <v>45459</v>
       </c>
       <c r="AK5" s="11">
         <f ca="1">AJ5+1</f>
-        <v>45453</v>
+        <v>45460</v>
       </c>
       <c r="AL5" s="10">
         <f ca="1">AK5+1</f>
-        <v>45454</v>
+        <v>45461</v>
       </c>
       <c r="AM5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45455</v>
+        <v>45462</v>
       </c>
       <c r="AN5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="AO5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45457</v>
+        <v>45464</v>
       </c>
       <c r="AP5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45458</v>
+        <v>45465</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="AR5" s="11">
         <f ca="1">AQ5+1</f>
-        <v>45460</v>
+        <v>45467</v>
       </c>
       <c r="AS5" s="10">
         <f ca="1">AR5+1</f>
-        <v>45461</v>
+        <v>45468</v>
       </c>
       <c r="AT5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45462</v>
+        <v>45469</v>
       </c>
       <c r="AU5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45463</v>
+        <v>45470</v>
       </c>
       <c r="AV5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45464</v>
+        <v>45471</v>
       </c>
       <c r="AW5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45465</v>
+        <v>45472</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45466</v>
+        <v>45473</v>
       </c>
       <c r="AY5" s="11">
         <f ca="1">AX5+1</f>
-        <v>45467</v>
+        <v>45474</v>
       </c>
       <c r="AZ5" s="10">
         <f ca="1">AY5+1</f>
-        <v>45468</v>
+        <v>45475</v>
       </c>
       <c r="BA5" s="10">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>45469</v>
+        <v>45476</v>
       </c>
       <c r="BB5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45470</v>
+        <v>45477</v>
       </c>
       <c r="BC5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45471</v>
+        <v>45478</v>
       </c>
       <c r="BD5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45472</v>
+        <v>45479</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" ca="1" si="1"/>
-        <v>45473</v>
+        <v>45480</v>
       </c>
       <c r="BF5" s="11">
         <f ca="1">BE5+1</f>
-        <v>45474</v>
+        <v>45481</v>
       </c>
       <c r="BG5" s="10">
         <f ca="1">BF5+1</f>
-        <v>45475</v>
+        <v>45482</v>
       </c>
       <c r="BH5" s="10">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>45476</v>
+        <v>45483</v>
       </c>
       <c r="BI5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45477</v>
+        <v>45484</v>
       </c>
       <c r="BJ5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45478</v>
+        <v>45485</v>
       </c>
       <c r="BK5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45479</v>
+        <v>45486</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" ca="1" si="2"/>
-        <v>45480</v>
+        <v>45487</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2300,11 +2300,11 @@
       </c>
       <c r="E9" s="66">
         <f ca="1">Project_Start</f>
-        <v>45429</v>
+        <v>45432</v>
       </c>
       <c r="F9" s="66">
         <f ca="1">Project_Start</f>
-        <v>45429</v>
+        <v>45432</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17">
@@ -2383,11 +2383,11 @@
       </c>
       <c r="E10" s="66">
         <f ca="1">F9</f>
-        <v>45429</v>
+        <v>45432</v>
       </c>
       <c r="F10" s="66">
         <f ca="1">E10+2</f>
-        <v>45431</v>
+        <v>45434</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17">
@@ -2464,11 +2464,11 @@
       </c>
       <c r="E11" s="66">
         <f ca="1">F10</f>
-        <v>45431</v>
+        <v>45434</v>
       </c>
       <c r="F11" s="66">
         <f ca="1">E11+4</f>
-        <v>45435</v>
+        <v>45438</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17">
@@ -2545,11 +2545,11 @@
       </c>
       <c r="E12" s="66">
         <f ca="1">F9</f>
-        <v>45429</v>
+        <v>45432</v>
       </c>
       <c r="F12" s="66">
         <f ca="1">E12+5</f>
-        <v>45434</v>
+        <v>45437</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="17">
@@ -3157,11 +3157,11 @@
       <c r="D20" s="32"/>
       <c r="E20" s="68">
         <f ca="1">E9+15</f>
-        <v>45444</v>
+        <v>45447</v>
       </c>
       <c r="F20" s="68">
         <f ca="1">E20+5</f>
-        <v>45449</v>
+        <v>45452</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="17">
@@ -3234,11 +3234,11 @@
       <c r="D21" s="32"/>
       <c r="E21" s="68">
         <f ca="1">F20+1</f>
-        <v>45450</v>
+        <v>45453</v>
       </c>
       <c r="F21" s="68">
         <f ca="1">E21+4</f>
-        <v>45454</v>
+        <v>45457</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17">
@@ -3311,11 +3311,11 @@
       <c r="D22" s="32"/>
       <c r="E22" s="68">
         <f ca="1">E21+5</f>
-        <v>45455</v>
+        <v>45458</v>
       </c>
       <c r="F22" s="68">
         <f ca="1">E22+5</f>
-        <v>45460</v>
+        <v>45463</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="17">
@@ -3388,11 +3388,11 @@
       <c r="D23" s="32"/>
       <c r="E23" s="68">
         <f ca="1">F22+1</f>
-        <v>45461</v>
+        <v>45464</v>
       </c>
       <c r="F23" s="68">
         <f ca="1">E23+4</f>
-        <v>45465</v>
+        <v>45468</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17">
@@ -3465,11 +3465,11 @@
       <c r="D24" s="32"/>
       <c r="E24" s="68">
         <f ca="1">E22</f>
-        <v>45455</v>
+        <v>45458</v>
       </c>
       <c r="F24" s="68">
         <f ca="1">E24+4</f>
-        <v>45459</v>
+        <v>45462</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="17">
@@ -4137,11 +4137,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4149,6 +4144,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D32">
     <cfRule type="dataBar" priority="14">
@@ -4378,15 +4378,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A6C24D38A47D4483BDD40956192BCF" ma:contentTypeVersion="39" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9f07f3829e5d09499baf2c8502db3ed1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="147d1278-e733-49aa-b400-ef7687d76ce3" xmlns:ns4="93d03e77-3551-4536-9208-3222abea9772" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae3c4703f3b8d4021d69f44788502e31" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4838,6 +4829,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4166818-70F8-4D06-AC57-4B3E04A31479}">
   <ds:schemaRefs>
@@ -4857,14 +4857,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02FA432F-35E5-44AC-838D-D2937AF03E34}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E51B8CD0-936E-4F4B-BD26-D0FCA6E1F434}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4882,4 +4874,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02FA432F-35E5-44AC-838D-D2937AF03E34}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>